<commit_message>
changed biosampleNumber to bioSampleNumber
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_01.06.20.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_01.06.20.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">harvester</t>
   </si>
   <si>
-    <t xml:space="preserve">biosampleNumber</t>
+    <t xml:space="preserve">bioSampleNumber</t>
   </si>
   <si>
     <t xml:space="preserve">experimentDesign</t>
@@ -123,6 +123,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -141,12 +147,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,11 +200,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -212,7 +216,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,10 +225,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -247,8 +247,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J56" activeCellId="0" sqref="J56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -257,20 +257,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -316,30 +316,30 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="G2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="8" t="n">
@@ -348,8 +348,8 @@
       <c r="L2" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
@@ -369,16 +369,16 @@
       <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="6" t="n">
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -390,8 +390,8 @@
       <c r="L3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -403,19 +403,19 @@
       <c r="C4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J4" s="7" t="s">
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="8" t="n">
@@ -424,8 +424,8 @@
       <c r="L4" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -434,19 +434,19 @@
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="6" t="n">
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -458,8 +458,8 @@
       <c r="L5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -471,19 +471,19 @@
       <c r="C6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J6" s="7" t="s">
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="8" t="n">
@@ -492,8 +492,8 @@
       <c r="L6" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -505,16 +505,16 @@
       <c r="C7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="6" t="n">
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -526,8 +526,8 @@
       <c r="L7" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -536,22 +536,22 @@
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J8" s="7" t="s">
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="8" t="n">
@@ -560,8 +560,8 @@
       <c r="L8" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -573,16 +573,16 @@
       <c r="C9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="6" t="n">
+      <c r="D9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -594,8 +594,8 @@
       <c r="L9" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -607,19 +607,19 @@
       <c r="C10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J10" s="7" t="s">
+      <c r="D10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K10" s="8" t="n">
@@ -628,8 +628,8 @@
       <c r="L10" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -638,19 +638,19 @@
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="6" t="n">
+      <c r="D11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -662,8 +662,8 @@
       <c r="L11" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -675,19 +675,19 @@
       <c r="C12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J12" s="7" t="s">
+      <c r="D12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K12" s="8" t="n">
@@ -696,8 +696,8 @@
       <c r="L12" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -709,16 +709,16 @@
       <c r="C13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="6" t="n">
+      <c r="D13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -730,8 +730,8 @@
       <c r="L13" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -740,22 +740,22 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J14" s="7" t="s">
+      <c r="C14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="8" t="n">
@@ -764,8 +764,8 @@
       <c r="L14" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -777,16 +777,16 @@
       <c r="C15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="6" t="n">
+      <c r="D15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -798,8 +798,8 @@
       <c r="L15" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -811,19 +811,19 @@
       <c r="C16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J16" s="7" t="s">
+      <c r="D16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K16" s="8" t="n">
@@ -832,8 +832,8 @@
       <c r="L16" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -842,19 +842,19 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="6" t="n">
+      <c r="C17" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
@@ -866,8 +866,8 @@
       <c r="L17" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -876,22 +876,22 @@
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="3" t="n">
-        <v>17</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="5" t="s">
+      <c r="C18" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J18" s="7" t="s">
+      <c r="H18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K18" s="8" t="n">
@@ -911,16 +911,16 @@
       <c r="C19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="D19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="6" t="n">
+      <c r="H19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
@@ -943,19 +943,19 @@
       <c r="C20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="5" t="s">
+      <c r="D20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J20" s="7" t="s">
+      <c r="H20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K20" s="8" t="n">
@@ -972,19 +972,19 @@
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="5" t="s">
+      <c r="C21" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="6" t="n">
+      <c r="H21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1007,19 +1007,19 @@
       <c r="C22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="D22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J22" s="7" t="s">
+      <c r="H22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K22" s="8" t="n">
@@ -1039,16 +1039,16 @@
       <c r="C23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="5" t="s">
+      <c r="D23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="6" t="n">
+      <c r="H23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
@@ -1068,22 +1068,22 @@
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="5" t="s">
+      <c r="D24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J24" s="7" t="s">
+      <c r="H24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K24" s="1" t="n">
@@ -1103,16 +1103,16 @@
       <c r="C25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="5" t="s">
+      <c r="D25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="6" t="n">
+      <c r="H25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J25" s="1" t="s">
@@ -1135,19 +1135,19 @@
       <c r="C26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="5" t="s">
+      <c r="D26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J26" s="7" t="s">
+      <c r="H26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K26" s="8" t="n">
@@ -1164,19 +1164,19 @@
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="5" t="s">
+      <c r="D27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="6" t="n">
+      <c r="H27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
@@ -1199,19 +1199,19 @@
       <c r="C28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="5" t="s">
+      <c r="D28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J28" s="7" t="s">
+      <c r="H28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K28" s="8" t="n">
@@ -1231,16 +1231,16 @@
       <c r="C29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="5" t="s">
+      <c r="D29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="6" t="n">
+      <c r="H29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
@@ -1260,22 +1260,22 @@
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="5" t="s">
+      <c r="D30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J30" s="7" t="s">
+      <c r="H30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K30" s="8" t="n">
@@ -1295,16 +1295,16 @@
       <c r="C31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="5" t="s">
+      <c r="D31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="6" t="n">
+      <c r="H31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
@@ -1327,19 +1327,19 @@
       <c r="C32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="5" t="s">
+      <c r="D32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J32" s="7" t="s">
+      <c r="H32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K32" s="8" t="n">
@@ -1356,19 +1356,19 @@
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="5" t="s">
+      <c r="D33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="6" t="n">
+      <c r="H33" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J33" s="1" t="s">
@@ -1388,22 +1388,22 @@
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="5" t="s">
+      <c r="D34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H34" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J34" s="7" t="s">
+      <c r="H34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K34" s="1" t="n">
@@ -1423,16 +1423,16 @@
       <c r="C35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="5" t="s">
+      <c r="D35" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H35" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="6" t="n">
+      <c r="H35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J35" s="1" t="s">
@@ -1455,19 +1455,19 @@
       <c r="C36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="5" t="s">
+      <c r="D36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J36" s="7" t="s">
+      <c r="H36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K36" s="8" t="n">
@@ -1484,19 +1484,19 @@
       <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="5" t="s">
+      <c r="D37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="6" t="n">
+      <c r="H37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J37" s="1" t="s">
@@ -1519,19 +1519,19 @@
       <c r="C38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J38" s="7" t="s">
+      <c r="D38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K38" s="8" t="n">
@@ -1551,16 +1551,16 @@
       <c r="C39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="6" t="n">
+      <c r="D39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J39" s="1" t="s">
@@ -1580,22 +1580,22 @@
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J40" s="7" t="s">
+      <c r="D40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K40" s="8" t="n">
@@ -1615,16 +1615,16 @@
       <c r="C41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="6" t="n">
+      <c r="D41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J41" s="1" t="s">
@@ -1647,19 +1647,19 @@
       <c r="C42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J42" s="7" t="s">
+      <c r="D42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J42" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K42" s="8" t="n">
@@ -1676,19 +1676,19 @@
       <c r="B43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="3" t="n">
+      <c r="C43" s="4" t="n">
         <v>42</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="6" t="n">
+      <c r="D43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J43" s="1" t="s">
@@ -1711,19 +1711,19 @@
       <c r="C44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J44" s="7" t="s">
+      <c r="D44" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J44" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K44" s="1" t="n">
@@ -1743,16 +1743,16 @@
       <c r="C45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" s="6" t="n">
+      <c r="D45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J45" s="1" t="s">
@@ -1772,22 +1772,22 @@
       <c r="B46" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="3" t="n">
+      <c r="C46" s="4" t="n">
         <v>45</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J46" s="7" t="s">
+      <c r="D46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J46" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K46" s="8" t="n">
@@ -1807,16 +1807,16 @@
       <c r="C47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" s="6" t="n">
+      <c r="D47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J47" s="1" t="s">
@@ -1839,19 +1839,19 @@
       <c r="C48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I48" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J48" s="7" t="s">
+      <c r="D48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J48" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K48" s="8" t="n">
@@ -1868,19 +1868,19 @@
       <c r="B49" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="3" t="n">
+      <c r="C49" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I49" s="6" t="n">
+      <c r="D49" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J49" s="1" t="s">
@@ -1900,22 +1900,22 @@
       <c r="B50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="3" t="n">
+      <c r="C50" s="4" t="n">
         <v>49</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I50" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J50" s="7" t="s">
+      <c r="D50" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J50" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K50" s="8" t="n">
@@ -1935,16 +1935,16 @@
       <c r="C51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I51" s="6" t="n">
+      <c r="D51" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J51" s="1" t="s">
@@ -1967,19 +1967,19 @@
       <c r="C52" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J52" s="7" t="s">
+      <c r="D52" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K52" s="8" t="n">
@@ -1996,19 +1996,19 @@
       <c r="B53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="3" t="n">
+      <c r="C53" s="4" t="n">
         <v>52</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I53" s="6" t="n">
+      <c r="D53" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J53" s="1" t="s">
@@ -2031,19 +2031,19 @@
       <c r="C54" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="D54" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I54" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J54" s="7" t="s">
+      <c r="D54" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K54" s="1" t="n">
@@ -2063,16 +2063,16 @@
       <c r="C55" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I55" s="6" t="n">
+      <c r="D55" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J55" s="1" t="s">
@@ -2092,22 +2092,22 @@
       <c r="B56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="3" t="n">
+      <c r="C56" s="4" t="n">
         <v>55</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I56" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="J56" s="7" t="s">
+      <c r="D56" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J56" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K56" s="8" t="n">
@@ -2127,16 +2127,16 @@
       <c r="C57" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I57" s="6" t="n">
+      <c r="D57" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="7" t="n">
         <v>30</v>
       </c>
       <c r="J57" s="1" t="s">

</xml_diff>

<commit_message>
modified the Cst6, Rgm1, Gal4, Rgt1 experiment sheets for all 5 replicates to fix key errors
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_01.06.20.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_01.06.20.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/bioSample/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431509A0-DA74-3342-9DC9-1CB0C497B333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-260" yWindow="460" windowWidth="18640" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -22,104 +35,84 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="21">
   <si>
-    <t xml:space="preserve">harvestDate</t>
+    <t>harvestDate</t>
   </si>
   <si>
-    <t xml:space="preserve">harvester</t>
+    <t>harvester</t>
   </si>
   <si>
-    <t xml:space="preserve">bioSampleNumber</t>
+    <t>bioSampleNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">experimentDesign</t>
+    <t>experimentDesign</t>
   </si>
   <si>
-    <t xml:space="preserve">experimentObservations</t>
+    <t>experimentObservations</t>
   </si>
   <si>
-    <t xml:space="preserve">strain</t>
+    <t>strain</t>
   </si>
   <si>
-    <t xml:space="preserve">genotype</t>
+    <t>genotype</t>
   </si>
   <si>
-    <t xml:space="preserve">floodmedia</t>
+    <t>floodmedia</t>
   </si>
   <si>
-    <t xml:space="preserve">inductionDelay</t>
+    <t>inductionDelay</t>
   </si>
   <si>
-    <t xml:space="preserve">treatment</t>
+    <t>treatment</t>
   </si>
   <si>
-    <t xml:space="preserve">timePoint</t>
+    <t>timePoint</t>
   </si>
   <si>
-    <t xml:space="preserve">replicate</t>
+    <t>replicate</t>
   </si>
   <si>
-    <t xml:space="preserve">01.06.20</t>
+    <t>01.06.20</t>
   </si>
   <si>
-    <t xml:space="preserve">J.PLAGGENBERG</t>
+    <t>J.PLAGGENBERG</t>
   </si>
   <si>
-    <t xml:space="preserve">ZEV_induction</t>
+    <t>ZEV_induction</t>
   </si>
   <si>
-    <t xml:space="preserve">TYE7</t>
+    <t>TYE7</t>
   </si>
   <si>
-    <t xml:space="preserve">SCGal</t>
+    <t>SCGal</t>
   </si>
   <si>
-    <t xml:space="preserve">EtOH</t>
+    <t>EtOH</t>
   </si>
   <si>
-    <t xml:space="preserve">Estradiol</t>
+    <t>Estradiol</t>
   </si>
   <si>
-    <t xml:space="preserve">CST6</t>
+    <t>CST6</t>
   </si>
   <si>
-    <t xml:space="preserve">RGM1</t>
+    <t>RGM1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -131,21 +124,18 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -158,7 +148,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -166,104 +156,360 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="14.43"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="6.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="14.5" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
+    <col min="12" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -315,14 +561,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -336,16 +582,16 @@
       <c r="H2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="7" t="n">
+      <c r="I2" s="7">
         <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="8" t="n">
+      <c r="K2" s="8">
         <v>-1</v>
       </c>
-      <c r="L2" s="8" t="n">
+      <c r="L2" s="8">
         <v>1</v>
       </c>
       <c r="P2" s="6"/>
@@ -359,14 +605,14 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -378,29 +624,29 @@
       <c r="H3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="7" t="n">
+      <c r="I3" s="7">
         <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="8" t="n">
+      <c r="K3" s="8">
         <v>-1</v>
       </c>
-      <c r="L3" s="8" t="n">
+      <c r="L3" s="8">
         <v>1</v>
       </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -412,29 +658,29 @@
       <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="7" t="n">
+      <c r="I4" s="7">
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L4" s="8" t="n">
+      <c r="K4" s="8">
+        <v>15</v>
+      </c>
+      <c r="L4" s="8">
         <v>1</v>
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="4">
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -446,29 +692,29 @@
       <c r="H5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="7">
         <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L5" s="8" t="n">
+      <c r="K5" s="8">
+        <v>15</v>
+      </c>
+      <c r="L5" s="8">
         <v>1</v>
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -480,29 +726,29 @@
       <c r="H6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="7" t="n">
+      <c r="I6" s="7">
         <v>30</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L6" s="8" t="n">
+      <c r="K6" s="8">
+        <v>20</v>
+      </c>
+      <c r="L6" s="8">
         <v>1</v>
       </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="1">
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -514,29 +760,29 @@
       <c r="H7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="7" t="n">
+      <c r="I7" s="7">
         <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L7" s="8" t="n">
+      <c r="K7" s="8">
+        <v>20</v>
+      </c>
+      <c r="L7" s="8">
         <v>1</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="4">
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -548,29 +794,29 @@
       <c r="H8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="7" t="n">
+      <c r="I8" s="7">
         <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="8" t="n">
+      <c r="K8" s="8">
         <v>90</v>
       </c>
-      <c r="L8" s="8" t="n">
+      <c r="L8" s="8">
         <v>1</v>
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="1">
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -582,29 +828,29 @@
       <c r="H9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="7" t="n">
+      <c r="I9" s="7">
         <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="8" t="n">
+      <c r="K9" s="8">
         <v>90</v>
       </c>
-      <c r="L9" s="8" t="n">
+      <c r="L9" s="8">
         <v>1</v>
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="1">
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -616,29 +862,29 @@
       <c r="H10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="7" t="n">
+      <c r="I10" s="7">
         <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="8" t="n">
+      <c r="K10" s="8">
         <v>-1</v>
       </c>
-      <c r="L10" s="8" t="n">
+      <c r="L10" s="8">
         <v>2</v>
       </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="C11" s="4">
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -650,29 +896,29 @@
       <c r="H11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="7" t="n">
+      <c r="I11" s="7">
         <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="8" t="n">
+      <c r="K11" s="8">
         <v>-1</v>
       </c>
-      <c r="L11" s="8" t="n">
+      <c r="L11" s="8">
         <v>2</v>
       </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="1">
         <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -684,29 +930,29 @@
       <c r="H12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="7" t="n">
+      <c r="I12" s="7">
         <v>30</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L12" s="8" t="n">
+      <c r="K12" s="8">
+        <v>15</v>
+      </c>
+      <c r="L12" s="8">
         <v>2</v>
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="1">
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -718,29 +964,29 @@
       <c r="H13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="7">
         <v>30</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L13" s="8" t="n">
+      <c r="K13" s="8">
+        <v>15</v>
+      </c>
+      <c r="L13" s="8">
         <v>2</v>
       </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="4" t="n">
+      <c r="C14" s="4">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -752,29 +998,29 @@
       <c r="H14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="7" t="n">
+      <c r="I14" s="7">
         <v>30</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L14" s="8" t="n">
+      <c r="K14" s="8">
+        <v>20</v>
+      </c>
+      <c r="L14" s="8">
         <v>2</v>
       </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="n">
+      <c r="C15" s="1">
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -786,29 +1032,29 @@
       <c r="H15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="7" t="n">
+      <c r="I15" s="7">
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L15" s="8" t="n">
+      <c r="K15" s="8">
+        <v>20</v>
+      </c>
+      <c r="L15" s="8">
         <v>2</v>
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="1">
         <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -820,29 +1066,29 @@
       <c r="H16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="7" t="n">
+      <c r="I16" s="7">
         <v>30</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="8" t="n">
+      <c r="K16" s="8">
         <v>90</v>
       </c>
-      <c r="L16" s="8" t="n">
+      <c r="L16" s="8">
         <v>2</v>
       </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="4" t="n">
+      <c r="C17" s="4">
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -854,29 +1100,29 @@
       <c r="H17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="7" t="n">
+      <c r="I17" s="7">
         <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="8" t="n">
+      <c r="K17" s="8">
         <v>90</v>
       </c>
-      <c r="L17" s="8" t="n">
+      <c r="L17" s="8">
         <v>2</v>
       </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="4" t="n">
+      <c r="C18" s="4">
         <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -888,27 +1134,27 @@
       <c r="H18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="7" t="n">
+      <c r="I18" s="7">
         <v>30</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="8" t="n">
+      <c r="K18" s="8">
         <v>-1</v>
       </c>
-      <c r="L18" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C19" s="1">
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -920,27 +1166,27 @@
       <c r="H19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="7" t="n">
+      <c r="I19" s="7">
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="8" t="n">
+      <c r="K19" s="8">
         <v>-1</v>
       </c>
-      <c r="L19" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="1">
         <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -952,27 +1198,27 @@
       <c r="H20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="7" t="n">
+      <c r="I20" s="7">
         <v>30</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L20" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K20" s="8">
+        <v>15</v>
+      </c>
+      <c r="L20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="4" t="n">
+      <c r="C21" s="4">
         <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -984,27 +1230,27 @@
       <c r="H21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="7" t="n">
+      <c r="I21" s="7">
         <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L21" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K21" s="8">
+        <v>15</v>
+      </c>
+      <c r="L21" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="1" t="n">
+      <c r="C22" s="1">
         <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1016,27 +1262,27 @@
       <c r="H22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="7" t="n">
+      <c r="I22" s="7">
         <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L22" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K22" s="8">
+        <v>20</v>
+      </c>
+      <c r="L22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="1" t="n">
+      <c r="C23" s="1">
         <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -1048,27 +1294,27 @@
       <c r="H23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="7" t="n">
+      <c r="I23" s="7">
         <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L23" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K23" s="8">
+        <v>20</v>
+      </c>
+      <c r="L23" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="4" t="n">
+      <c r="C24" s="4">
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -1080,27 +1326,27 @@
       <c r="H24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="7" t="n">
+      <c r="I24" s="7">
         <v>30</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="L24" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K24" s="1">
+        <v>30</v>
+      </c>
+      <c r="L24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="1" t="n">
+      <c r="C25" s="1">
         <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -1112,27 +1358,27 @@
       <c r="H25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="7" t="n">
+      <c r="I25" s="7">
         <v>30</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="L25" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K25" s="1">
+        <v>30</v>
+      </c>
+      <c r="L25" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="1" t="n">
+      <c r="C26" s="1">
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -1144,27 +1390,27 @@
       <c r="H26" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="7" t="n">
+      <c r="I26" s="7">
         <v>30</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="8" t="n">
+      <c r="K26" s="8">
         <v>90</v>
       </c>
-      <c r="L26" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="4" t="n">
+      <c r="C27" s="4">
         <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -1176,27 +1422,27 @@
       <c r="H27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="7" t="n">
+      <c r="I27" s="7">
         <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K27" s="8" t="n">
+      <c r="K27" s="8">
         <v>90</v>
       </c>
-      <c r="L27" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="1" t="n">
+      <c r="C28" s="1">
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -1208,27 +1454,27 @@
       <c r="H28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="7" t="n">
+      <c r="I28" s="7">
         <v>30</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="8" t="n">
+      <c r="K28" s="8">
         <v>-1</v>
       </c>
-      <c r="L28" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L28" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="1" t="n">
+      <c r="C29" s="1">
         <v>28</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -1240,27 +1486,27 @@
       <c r="H29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="7" t="n">
+      <c r="I29" s="7">
         <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="8" t="n">
+      <c r="K29" s="8">
         <v>-1</v>
       </c>
-      <c r="L29" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L29" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="4" t="n">
+      <c r="C30" s="4">
         <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -1272,27 +1518,27 @@
       <c r="H30" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="7" t="n">
+      <c r="I30" s="7">
         <v>30</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L30" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K30" s="8">
+        <v>15</v>
+      </c>
+      <c r="L30" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="1" t="n">
+      <c r="C31" s="1">
         <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -1304,27 +1550,27 @@
       <c r="H31" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="7" t="n">
+      <c r="I31" s="7">
         <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K31" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L31" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K31" s="8">
+        <v>15</v>
+      </c>
+      <c r="L31" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="1" t="n">
+      <c r="C32" s="1">
         <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -1336,27 +1582,27 @@
       <c r="H32" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="7" t="n">
+      <c r="I32" s="7">
         <v>30</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L32" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K32" s="8">
+        <v>20</v>
+      </c>
+      <c r="L32" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="4" t="n">
+      <c r="C33" s="4">
         <v>32</v>
       </c>
       <c r="D33" s="5" t="s">
@@ -1368,27 +1614,27 @@
       <c r="H33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="7" t="n">
+      <c r="I33" s="7">
         <v>30</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L33" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K33" s="8">
+        <v>20</v>
+      </c>
+      <c r="L33" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="4" t="n">
+      <c r="C34" s="4">
         <v>33</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -1400,27 +1646,27 @@
       <c r="H34" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="7" t="n">
+      <c r="I34" s="7">
         <v>30</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K34" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="L34" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K34" s="1">
+        <v>30</v>
+      </c>
+      <c r="L34" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="1" t="n">
+      <c r="C35" s="1">
         <v>34</v>
       </c>
       <c r="D35" s="5" t="s">
@@ -1432,27 +1678,27 @@
       <c r="H35" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="7" t="n">
+      <c r="I35" s="7">
         <v>30</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K35" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="L35" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K35" s="1">
+        <v>30</v>
+      </c>
+      <c r="L35" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="1" t="n">
+      <c r="C36" s="1">
         <v>35</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -1464,27 +1710,27 @@
       <c r="H36" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="7" t="n">
+      <c r="I36" s="7">
         <v>30</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K36" s="8" t="n">
+      <c r="K36" s="8">
         <v>90</v>
       </c>
-      <c r="L36" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="4" t="n">
+      <c r="C37" s="4">
         <v>36</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -1496,27 +1742,27 @@
       <c r="H37" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I37" s="7" t="n">
+      <c r="I37" s="7">
         <v>30</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K37" s="8" t="n">
+      <c r="K37" s="8">
         <v>90</v>
       </c>
-      <c r="L37" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L37" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="1" t="n">
+      <c r="C38" s="1">
         <v>37</v>
       </c>
       <c r="D38" s="5" t="s">
@@ -1528,27 +1774,27 @@
       <c r="H38" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I38" s="7" t="n">
+      <c r="I38" s="7">
         <v>30</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="8" t="n">
+      <c r="K38" s="8">
         <v>-1</v>
       </c>
-      <c r="L38" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L38" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="1" t="n">
+      <c r="C39" s="1">
         <v>38</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -1560,27 +1806,27 @@
       <c r="H39" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="7" t="n">
+      <c r="I39" s="7">
         <v>30</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K39" s="8" t="n">
+      <c r="K39" s="8">
         <v>-1</v>
       </c>
-      <c r="L39" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L39" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="4" t="n">
+      <c r="C40" s="4">
         <v>39</v>
       </c>
       <c r="D40" s="5" t="s">
@@ -1592,27 +1838,27 @@
       <c r="H40" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="7" t="n">
+      <c r="I40" s="7">
         <v>30</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K40" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L40" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K40" s="8">
+        <v>15</v>
+      </c>
+      <c r="L40" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="1" t="n">
+      <c r="C41" s="1">
         <v>40</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -1624,27 +1870,27 @@
       <c r="H41" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I41" s="7" t="n">
+      <c r="I41" s="7">
         <v>30</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K41" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L41" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K41" s="8">
+        <v>15</v>
+      </c>
+      <c r="L41" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="1" t="n">
+      <c r="C42" s="1">
         <v>41</v>
       </c>
       <c r="D42" s="5" t="s">
@@ -1656,27 +1902,27 @@
       <c r="H42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I42" s="7" t="n">
+      <c r="I42" s="7">
         <v>30</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K42" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L42" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K42" s="8">
+        <v>20</v>
+      </c>
+      <c r="L42" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="4" t="n">
+      <c r="C43" s="4">
         <v>42</v>
       </c>
       <c r="D43" s="5" t="s">
@@ -1688,27 +1934,27 @@
       <c r="H43" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I43" s="7" t="n">
+      <c r="I43" s="7">
         <v>30</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K43" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L43" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K43" s="8">
+        <v>20</v>
+      </c>
+      <c r="L43" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="1" t="n">
+      <c r="C44" s="1">
         <v>43</v>
       </c>
       <c r="D44" s="5" t="s">
@@ -1720,27 +1966,27 @@
       <c r="H44" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I44" s="7" t="n">
+      <c r="I44" s="7">
         <v>30</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K44" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="L44" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K44" s="1">
+        <v>30</v>
+      </c>
+      <c r="L44" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="1" t="n">
+      <c r="C45" s="1">
         <v>44</v>
       </c>
       <c r="D45" s="5" t="s">
@@ -1752,27 +1998,27 @@
       <c r="H45" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I45" s="7" t="n">
+      <c r="I45" s="7">
         <v>30</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K45" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="L45" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K45" s="1">
+        <v>30</v>
+      </c>
+      <c r="L45" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="4" t="n">
+      <c r="C46" s="4">
         <v>45</v>
       </c>
       <c r="D46" s="5" t="s">
@@ -1784,27 +2030,27 @@
       <c r="H46" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I46" s="7" t="n">
+      <c r="I46" s="7">
         <v>30</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K46" s="8" t="n">
+      <c r="K46" s="8">
         <v>90</v>
       </c>
-      <c r="L46" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="1" t="n">
+      <c r="C47" s="1">
         <v>46</v>
       </c>
       <c r="D47" s="5" t="s">
@@ -1816,27 +2062,27 @@
       <c r="H47" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I47" s="7" t="n">
+      <c r="I47" s="7">
         <v>30</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K47" s="8" t="n">
+      <c r="K47" s="8">
         <v>90</v>
       </c>
-      <c r="L47" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="1" t="n">
+      <c r="C48" s="1">
         <v>47</v>
       </c>
       <c r="D48" s="5" t="s">
@@ -1848,27 +2094,27 @@
       <c r="H48" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I48" s="7" t="n">
+      <c r="I48" s="7">
         <v>30</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K48" s="8" t="n">
+      <c r="K48" s="8">
         <v>-1</v>
       </c>
-      <c r="L48" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L48" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="4" t="n">
+      <c r="C49" s="4">
         <v>48</v>
       </c>
       <c r="D49" s="5" t="s">
@@ -1880,27 +2126,27 @@
       <c r="H49" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I49" s="7" t="n">
+      <c r="I49" s="7">
         <v>30</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K49" s="8" t="n">
+      <c r="K49" s="8">
         <v>-1</v>
       </c>
-      <c r="L49" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L49" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="4" t="n">
+      <c r="C50" s="4">
         <v>49</v>
       </c>
       <c r="D50" s="5" t="s">
@@ -1912,27 +2158,27 @@
       <c r="H50" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I50" s="7" t="n">
+      <c r="I50" s="7">
         <v>30</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K50" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L50" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K50" s="8">
+        <v>15</v>
+      </c>
+      <c r="L50" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="1" t="n">
+      <c r="C51" s="1">
         <v>50</v>
       </c>
       <c r="D51" s="5" t="s">
@@ -1944,27 +2190,27 @@
       <c r="H51" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I51" s="7" t="n">
+      <c r="I51" s="7">
         <v>30</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K51" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="L51" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K51" s="8">
+        <v>15</v>
+      </c>
+      <c r="L51" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C52" s="1" t="n">
+      <c r="C52" s="1">
         <v>51</v>
       </c>
       <c r="D52" s="5" t="s">
@@ -1976,27 +2222,27 @@
       <c r="H52" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I52" s="7" t="n">
+      <c r="I52" s="7">
         <v>30</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K52" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L52" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K52" s="8">
+        <v>20</v>
+      </c>
+      <c r="L52" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="4" t="n">
+      <c r="C53" s="4">
         <v>52</v>
       </c>
       <c r="D53" s="5" t="s">
@@ -2008,27 +2254,27 @@
       <c r="H53" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I53" s="7" t="n">
+      <c r="I53" s="7">
         <v>30</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K53" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="L53" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K53" s="8">
+        <v>20</v>
+      </c>
+      <c r="L53" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C54" s="1" t="n">
+      <c r="C54" s="1">
         <v>53</v>
       </c>
       <c r="D54" s="5" t="s">
@@ -2040,27 +2286,27 @@
       <c r="H54" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I54" s="7" t="n">
+      <c r="I54" s="7">
         <v>30</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K54" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="L54" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K54" s="1">
+        <v>30</v>
+      </c>
+      <c r="L54" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="1" t="n">
+      <c r="C55" s="1">
         <v>54</v>
       </c>
       <c r="D55" s="5" t="s">
@@ -2072,27 +2318,27 @@
       <c r="H55" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I55" s="7" t="n">
+      <c r="I55" s="7">
         <v>30</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K55" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="L55" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K55" s="1">
+        <v>30</v>
+      </c>
+      <c r="L55" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="4" t="n">
+      <c r="C56" s="4">
         <v>55</v>
       </c>
       <c r="D56" s="5" t="s">
@@ -2104,27 +2350,27 @@
       <c r="H56" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I56" s="7" t="n">
+      <c r="I56" s="7">
         <v>30</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K56" s="8" t="n">
+      <c r="K56" s="8">
         <v>90</v>
       </c>
-      <c r="L56" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="1" t="n">
+      <c r="C57" s="1">
         <v>56</v>
       </c>
       <c r="D57" s="5" t="s">
@@ -2136,27 +2382,22 @@
       <c r="H57" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I57" s="7" t="n">
+      <c r="I57" s="7">
         <v>30</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K57" s="8" t="n">
+      <c r="K57" s="8">
         <v>90</v>
       </c>
-      <c r="L57" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="L57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
editing ZEV biosample sheets to correct treatment column; EtOH vs mockEstradiol
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_01.06.20.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_01.06.20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431509A0-DA74-3342-9DC9-1CB0C497B333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC41532-CCA0-E64B-B516-822EAE9FA317}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-260" yWindow="460" windowWidth="18640" windowHeight="20040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10180" yWindow="460" windowWidth="22980" windowHeight="19840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>SCGal</t>
   </si>
   <si>
-    <t>EtOH</t>
-  </si>
-  <si>
     <t>Estradiol</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>RGM1</t>
+  </si>
+  <si>
+    <t>mockEstradiol</t>
   </si>
 </sst>
 </file>
@@ -113,7 +113,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -124,19 +124,19 @@
     <font>
       <sz val="11"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -491,20 +491,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:C47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="14.5" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="6.5" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="14.5" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="13" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" customWidth="1"/>
     <col min="11" max="11" width="9.83203125" customWidth="1"/>
     <col min="12" max="1025" width="14.5" customWidth="1"/>
   </cols>
@@ -586,13 +584,13 @@
         <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K2" s="8">
         <v>-1</v>
       </c>
       <c r="L2" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -628,13 +626,13 @@
         <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" s="8">
         <v>-1</v>
       </c>
       <c r="L3" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -662,13 +660,13 @@
         <v>30</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K4" s="8">
         <v>15</v>
       </c>
       <c r="L4" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
@@ -696,13 +694,13 @@
         <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5" s="8">
         <v>15</v>
       </c>
       <c r="L5" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -730,13 +728,13 @@
         <v>30</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K6" s="8">
         <v>20</v>
       </c>
       <c r="L6" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -764,13 +762,13 @@
         <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" s="8">
         <v>20</v>
       </c>
       <c r="L7" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -798,13 +796,13 @@
         <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K8" s="8">
         <v>90</v>
       </c>
       <c r="L8" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
@@ -832,13 +830,13 @@
         <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="8">
         <v>90</v>
       </c>
       <c r="L9" s="8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
@@ -866,13 +864,13 @@
         <v>30</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K10" s="8">
         <v>-1</v>
       </c>
       <c r="L10" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
@@ -900,13 +898,13 @@
         <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K11" s="8">
         <v>-1</v>
       </c>
       <c r="L11" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -934,13 +932,13 @@
         <v>30</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K12" s="8">
         <v>15</v>
       </c>
       <c r="L12" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
@@ -968,13 +966,13 @@
         <v>30</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K13" s="8">
         <v>15</v>
       </c>
       <c r="L13" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
@@ -1002,13 +1000,13 @@
         <v>30</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K14" s="8">
         <v>20</v>
       </c>
       <c r="L14" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
@@ -1036,13 +1034,13 @@
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K15" s="8">
         <v>20</v>
       </c>
       <c r="L15" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
@@ -1070,13 +1068,13 @@
         <v>30</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K16" s="8">
         <v>90</v>
       </c>
       <c r="L16" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
@@ -1104,13 +1102,13 @@
         <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K17" s="8">
         <v>90</v>
       </c>
       <c r="L17" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
@@ -1129,7 +1127,7 @@
         <v>14</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>16</v>
@@ -1138,7 +1136,7 @@
         <v>30</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K18" s="8">
         <v>-1</v>
@@ -1161,7 +1159,7 @@
         <v>14</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>16</v>
@@ -1170,7 +1168,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K19" s="8">
         <v>-1</v>
@@ -1193,7 +1191,7 @@
         <v>14</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>16</v>
@@ -1202,7 +1200,7 @@
         <v>30</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K20" s="8">
         <v>15</v>
@@ -1225,7 +1223,7 @@
         <v>14</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>16</v>
@@ -1234,7 +1232,7 @@
         <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K21" s="8">
         <v>15</v>
@@ -1257,7 +1255,7 @@
         <v>14</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>16</v>
@@ -1266,7 +1264,7 @@
         <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K22" s="8">
         <v>20</v>
@@ -1289,7 +1287,7 @@
         <v>14</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>16</v>
@@ -1298,7 +1296,7 @@
         <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K23" s="8">
         <v>20</v>
@@ -1321,7 +1319,7 @@
         <v>14</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>16</v>
@@ -1330,7 +1328,7 @@
         <v>30</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K24" s="1">
         <v>30</v>
@@ -1353,7 +1351,7 @@
         <v>14</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>16</v>
@@ -1362,7 +1360,7 @@
         <v>30</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K25" s="1">
         <v>30</v>
@@ -1385,7 +1383,7 @@
         <v>14</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>16</v>
@@ -1394,7 +1392,7 @@
         <v>30</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K26" s="8">
         <v>90</v>
@@ -1417,7 +1415,7 @@
         <v>14</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>16</v>
@@ -1426,7 +1424,7 @@
         <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K27" s="8">
         <v>90</v>
@@ -1449,7 +1447,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>16</v>
@@ -1458,7 +1456,7 @@
         <v>30</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K28" s="8">
         <v>-1</v>
@@ -1481,7 +1479,7 @@
         <v>14</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>16</v>
@@ -1490,7 +1488,7 @@
         <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K29" s="8">
         <v>-1</v>
@@ -1513,7 +1511,7 @@
         <v>14</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>16</v>
@@ -1522,7 +1520,7 @@
         <v>30</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K30" s="8">
         <v>15</v>
@@ -1545,7 +1543,7 @@
         <v>14</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>16</v>
@@ -1554,7 +1552,7 @@
         <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K31" s="8">
         <v>15</v>
@@ -1577,7 +1575,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>16</v>
@@ -1586,7 +1584,7 @@
         <v>30</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K32" s="8">
         <v>20</v>
@@ -1609,7 +1607,7 @@
         <v>14</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>16</v>
@@ -1618,7 +1616,7 @@
         <v>30</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K33" s="8">
         <v>20</v>
@@ -1641,7 +1639,7 @@
         <v>14</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>16</v>
@@ -1650,7 +1648,7 @@
         <v>30</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K34" s="1">
         <v>30</v>
@@ -1673,7 +1671,7 @@
         <v>14</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>16</v>
@@ -1682,7 +1680,7 @@
         <v>30</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K35" s="1">
         <v>30</v>
@@ -1705,7 +1703,7 @@
         <v>14</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>16</v>
@@ -1714,7 +1712,7 @@
         <v>30</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K36" s="8">
         <v>90</v>
@@ -1737,7 +1735,7 @@
         <v>14</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>16</v>
@@ -1746,7 +1744,7 @@
         <v>30</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K37" s="8">
         <v>90</v>
@@ -1769,7 +1767,7 @@
         <v>14</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>16</v>
@@ -1778,7 +1776,7 @@
         <v>30</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K38" s="8">
         <v>-1</v>
@@ -1801,7 +1799,7 @@
         <v>14</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>16</v>
@@ -1810,7 +1808,7 @@
         <v>30</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K39" s="8">
         <v>-1</v>
@@ -1833,7 +1831,7 @@
         <v>14</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>16</v>
@@ -1842,7 +1840,7 @@
         <v>30</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K40" s="8">
         <v>15</v>
@@ -1865,7 +1863,7 @@
         <v>14</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>16</v>
@@ -1874,7 +1872,7 @@
         <v>30</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K41" s="8">
         <v>15</v>
@@ -1897,7 +1895,7 @@
         <v>14</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>16</v>
@@ -1906,7 +1904,7 @@
         <v>30</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K42" s="8">
         <v>20</v>
@@ -1929,7 +1927,7 @@
         <v>14</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>16</v>
@@ -1938,7 +1936,7 @@
         <v>30</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K43" s="8">
         <v>20</v>
@@ -1961,7 +1959,7 @@
         <v>14</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>16</v>
@@ -1970,7 +1968,7 @@
         <v>30</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K44" s="1">
         <v>30</v>
@@ -1993,7 +1991,7 @@
         <v>14</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>16</v>
@@ -2002,7 +2000,7 @@
         <v>30</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K45" s="1">
         <v>30</v>
@@ -2025,7 +2023,7 @@
         <v>14</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>16</v>
@@ -2034,7 +2032,7 @@
         <v>30</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K46" s="8">
         <v>90</v>
@@ -2057,7 +2055,7 @@
         <v>14</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>16</v>
@@ -2066,7 +2064,7 @@
         <v>30</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K47" s="8">
         <v>90</v>
@@ -2089,7 +2087,7 @@
         <v>14</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>16</v>
@@ -2098,7 +2096,7 @@
         <v>30</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K48" s="8">
         <v>-1</v>
@@ -2121,7 +2119,7 @@
         <v>14</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>16</v>
@@ -2130,7 +2128,7 @@
         <v>30</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K49" s="8">
         <v>-1</v>
@@ -2153,7 +2151,7 @@
         <v>14</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>16</v>
@@ -2162,7 +2160,7 @@
         <v>30</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K50" s="8">
         <v>15</v>
@@ -2185,7 +2183,7 @@
         <v>14</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>16</v>
@@ -2194,7 +2192,7 @@
         <v>30</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K51" s="8">
         <v>15</v>
@@ -2217,7 +2215,7 @@
         <v>14</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>16</v>
@@ -2226,7 +2224,7 @@
         <v>30</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K52" s="8">
         <v>20</v>
@@ -2249,7 +2247,7 @@
         <v>14</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>16</v>
@@ -2258,7 +2256,7 @@
         <v>30</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K53" s="8">
         <v>20</v>
@@ -2281,7 +2279,7 @@
         <v>14</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>16</v>
@@ -2290,7 +2288,7 @@
         <v>30</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K54" s="1">
         <v>30</v>
@@ -2313,7 +2311,7 @@
         <v>14</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>16</v>
@@ -2322,7 +2320,7 @@
         <v>30</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K55" s="1">
         <v>30</v>
@@ -2345,7 +2343,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>16</v>
@@ -2354,7 +2352,7 @@
         <v>30</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K56" s="8">
         <v>90</v>
@@ -2377,7 +2375,7 @@
         <v>14</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>16</v>
@@ -2386,7 +2384,7 @@
         <v>30</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K57" s="8">
         <v>90</v>

</xml_diff>